<commit_message>
Adicionado dados com a planilha
</commit_message>
<xml_diff>
--- a/BDjheniferdoce.xlsx
+++ b/BDjheniferdoce.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davip\OneDrive\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davip\OneDrive\Documentos\doceriajhenifersouza\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3788D3B-A249-43F5-B150-C4A7C800ADB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6B0DD9-DE5E-4415-B362-AC63E7D6CFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{982BB75A-ACDA-4BBD-AA99-4087C8B2A75F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Produtos" sheetId="1" r:id="rId1"/>
@@ -18,17 +18,12 @@
     <sheet name="Pedidos" sheetId="3" r:id="rId3"/>
     <sheet name="Clientes" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="57">
   <si>
     <t>Produto</t>
   </si>
@@ -36,32 +31,200 @@
     <t>Preço</t>
   </si>
   <si>
-    <t>teste</t>
+    <t>big copo duplo ninho morango</t>
+  </si>
+  <si>
+    <t>R$19.00</t>
+  </si>
+  <si>
+    <t>big copo ferreiro</t>
+  </si>
+  <si>
+    <t>big copo ninho + nutella</t>
+  </si>
+  <si>
+    <t>bolo bom bom de morango</t>
+  </si>
+  <si>
+    <t>R$15.00</t>
+  </si>
+  <si>
+    <t>bolo pote chocolatudo</t>
+  </si>
+  <si>
+    <t>R$14.00</t>
+  </si>
+  <si>
+    <t>bolo pote ninho com nutella</t>
+  </si>
+  <si>
+    <t>bolo pote prestigio</t>
+  </si>
+  <si>
+    <t>R$13.00</t>
+  </si>
+  <si>
+    <t>bolo pote red velvet</t>
+  </si>
+  <si>
+    <t>bolo vulcão</t>
+  </si>
+  <si>
+    <t>R$29.00</t>
+  </si>
+  <si>
+    <t>copo dois amores</t>
+  </si>
+  <si>
+    <t>R$18.00</t>
+  </si>
+  <si>
+    <t>coxinha carne de sol</t>
+  </si>
+  <si>
+    <t>R$9.50</t>
+  </si>
+  <si>
+    <t>coxinha frango catupiry</t>
+  </si>
+  <si>
+    <t>R$8.00</t>
+  </si>
+  <si>
+    <t>delicia de abacaxi</t>
+  </si>
+  <si>
+    <t>R$12.00</t>
+  </si>
+  <si>
+    <t>duplo ninho geleia de morango</t>
+  </si>
+  <si>
+    <t>empadão</t>
+  </si>
+  <si>
+    <t>fatia brownie morango</t>
+  </si>
+  <si>
+    <t>fatia brownie ninho+nutella</t>
+  </si>
+  <si>
+    <t>R$12.50</t>
+  </si>
+  <si>
+    <t>Pão de frongo com catupiry</t>
+  </si>
+  <si>
+    <t>R$10.00</t>
+  </si>
+  <si>
+    <t>Pão pizza</t>
+  </si>
+  <si>
+    <t>pudim</t>
+  </si>
+  <si>
+    <t>R$8.50</t>
+  </si>
+  <si>
+    <t>sanduba brownie bem casado</t>
+  </si>
+  <si>
+    <t>R$9.00</t>
+  </si>
+  <si>
+    <t>sanduba brownie ninho</t>
+  </si>
+  <si>
+    <t>sanduba brownie nutella</t>
+  </si>
+  <si>
+    <t>torta de limao</t>
+  </si>
+  <si>
+    <t>trufado de maracuja</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>caete 2</t>
+  </si>
+  <si>
+    <t>caetes 1</t>
+  </si>
+  <si>
+    <t>planalto</t>
+  </si>
+  <si>
+    <t>caetes 3</t>
+  </si>
+  <si>
+    <t>abreu centro</t>
+  </si>
+  <si>
+    <t>desterro</t>
+  </si>
+  <si>
+    <t>matinha</t>
+  </si>
+  <si>
+    <t>fosfato</t>
+  </si>
+  <si>
+    <t>cruz de rebouça</t>
+  </si>
+  <si>
+    <t>igarassu</t>
+  </si>
+  <si>
+    <t>paratibe</t>
+  </si>
+  <si>
+    <t>arthur 1</t>
+  </si>
+  <si>
+    <t>arthur 2</t>
+  </si>
+  <si>
+    <t>paulista centro</t>
+  </si>
+  <si>
+    <t>matranguape 1</t>
+  </si>
+  <si>
+    <t>torre galvão</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFCCCCCC"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,23 +244,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -405,97 +566,423 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D26FC32-324E-4554-BA17-29AF2D6A5F18}">
-  <dimension ref="A1:B9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1:B27" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21936916-F4C8-4958-8023-F75216796E9E}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
+    <sortCondition ref="A2:A17"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BB0D471-86F9-49A7-8998-9E4CDA22E5A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{617E3334-803A-478B-B9EE-FB8154A91797}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>